<commit_message>
added icons to keys and minor formatting updates
</commit_message>
<xml_diff>
--- a/general_cities.xlsx
+++ b/general_cities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cadenlin/PycharmProjects/heatmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636987B5-13F2-8041-BA7D-DD990C7ABBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EC2C65-E5ED-664D-931C-8DDEA1DFDA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36040" yWindow="500" windowWidth="31160" windowHeight="21100" activeTab="6" xr2:uid="{AF0BBA4D-6ACA-7845-BC9B-0D28D119FCBA}"/>
+    <workbookView xWindow="36040" yWindow="500" windowWidth="31160" windowHeight="21100" activeTab="7" xr2:uid="{AF0BBA4D-6ACA-7845-BC9B-0D28D119FCBA}"/>
   </bookViews>
   <sheets>
     <sheet name="McCain" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Temple" sheetId="5" r:id="rId5"/>
     <sheet name="Oriux" sheetId="6" r:id="rId6"/>
     <sheet name="Western Systems" sheetId="7" r:id="rId7"/>
-    <sheet name="Mobotrex" sheetId="8" r:id="rId8"/>
+    <sheet name="MoboTrex" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
@@ -682,7 +682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D232B2-E1F3-3A42-92D0-0E689F892683}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
@@ -784,7 +784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C8684A-60BB-434A-819C-263F29ABE04E}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>